<commit_message>
added additional cmax results
</commit_message>
<xml_diff>
--- a/experiments/11_sched_method_comparison_6/Cmax.xlsx
+++ b/experiments/11_sched_method_comparison_6/Cmax.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\DP\experiments\11_sched_method_comparison_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033362D1-904F-40A2-A881-50E5BCBF9033}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB84F31F-0D33-4FB9-8B3C-EF357EF4F51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0DDFCFBD-5BFA-484A-9640-7E9D9F2D067B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>Run 1</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Mod.2 B Predictor</t>
+  </si>
+  <si>
+    <t>Mod.2 B Predictor - 930ms solution</t>
+  </si>
+  <si>
+    <t>min util LTF</t>
   </si>
 </sst>
 </file>
@@ -576,11 +582,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$37</c:f>
+              <c:f>Sheet1!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average</c:v>
+                  <c:v>Mod.2 B Predictor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -724,6 +730,264 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9E0C-4884-BE41-BEA923A045DE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B Predictor - 930ms solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$48:$F$53</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>1.0555066187486566</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.64538842740029267</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.511823622869634</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.6025013780545301</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.2456241630425897</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1356540944417113</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$48:$F$53</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>1.0555066187486566</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.64538842740029267</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.511823622869634</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.6025013780545301</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.2456241630425897</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1356540944417113</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$48:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>61.138666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.229333333333329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.120000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.688000000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.31133333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.337333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FE7-49E6-9B50-2C0AF52BF76D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>min util LTF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$58:$F$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0.34820683508512562</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.86289023378153829</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.92865111257613508</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.63523503961569761</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.49530058213842942</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.36582448736457523</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$58:$F$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0.34820683508512562</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.86289023378153829</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.92865111257613508</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.63523503961569761</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.49530058213842942</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.36582448736457523</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$58:$E$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>61.731999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.806666666666672</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.405333333333338</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.489333333333342</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.196000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.945333333333338</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4FE7-49E6-9B50-2C0AF52BF76D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -980,6 +1244,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1099,11 +1394,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$37</c:f>
+              <c:f>Sheet1!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average</c:v>
+                  <c:v>Mod.2 B Predictor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1247,6 +1542,264 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BBF5-4196-A2AC-70E31A4B1487}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B Predictor - 930ms solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$K$48:$K$53</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0.29362144941328017</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.70288584184538994</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.14026378324030128</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.9688497961927335E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.13292474061161907</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.2031350508624476</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$K$48:$K$53</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0.29362144941328017</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.70288584184538994</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.14026378324030128</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.9688497961927335E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.13292474061161907</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.2031350508624476</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$48:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>36.812333333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.463400000000036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.301866666666704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.686000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.7332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.902466666666669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F32-43F6-B67E-4EB27CABFB2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>min util LTF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$K$58:$K$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0.12175618624484398</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.18653145102695695</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.26223705984391144</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.10802596395723466</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.11319803688915357</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.4316839036922746E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$K$58:$K$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0.12175618624484398</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.18653145102695695</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.26223705984391144</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.10802596395723466</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.11319803688915357</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.4316839036922746E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$58:$J$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>37.576733333333337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.526333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.111333333333363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.263133333333336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0478666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.8356666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9F32-43F6-B67E-4EB27CABFB2E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1504,6 +2057,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3003,7 +3587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7020C77-4E36-4B3B-AB3A-E3315EA6D905}">
-  <dimension ref="A35:O53"/>
+  <dimension ref="A35:Y63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
@@ -3012,15 +3596,20 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="24" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="35" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="P35" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="40" t="s">
         <v>3</v>
@@ -3041,8 +3630,24 @@
       </c>
       <c r="M36" s="38"/>
       <c r="N36" s="39"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="R36" s="38"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="U36" s="38"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="X36" s="38"/>
+      <c r="Y36" s="39"/>
     </row>
-    <row r="37" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>8</v>
       </c>
@@ -3085,8 +3690,38 @@
       <c r="N37" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="P37" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S37" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V37" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="W37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y37" s="27" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="38" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>930</v>
       </c>
@@ -3136,8 +3771,45 @@
       <c r="N38" s="13">
         <v>23.0152</v>
       </c>
+      <c r="P38" s="22">
+        <v>930</v>
+      </c>
+      <c r="Q38" s="28">
+        <f>4*P38</f>
+        <v>3720</v>
+      </c>
+      <c r="R38" s="28">
+        <f>2*P38</f>
+        <v>1860</v>
+      </c>
+      <c r="S38" s="29">
+        <f>Q38+R38</f>
+        <v>5580</v>
+      </c>
+      <c r="T38" s="28">
+        <v>2964</v>
+      </c>
+      <c r="U38" s="28">
+        <v>1264</v>
+      </c>
+      <c r="V38" s="29">
+        <f>T38+U38</f>
+        <v>4228</v>
+      </c>
+      <c r="W38" s="30">
+        <f>T38/Q38</f>
+        <v>0.79677419354838708</v>
+      </c>
+      <c r="X38" s="30">
+        <f>U38/R38</f>
+        <v>0.67956989247311828</v>
+      </c>
+      <c r="Y38" s="31">
+        <f>V38/S38</f>
+        <v>0.75770609318996418</v>
+      </c>
     </row>
-    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <v>1130</v>
       </c>
@@ -3188,8 +3860,45 @@
         <v>23.403199999999998</v>
       </c>
       <c r="O39" s="36"/>
+      <c r="P39" s="22">
+        <v>1130</v>
+      </c>
+      <c r="Q39" s="28">
+        <f t="shared" ref="Q39:Q43" si="5">4*P39</f>
+        <v>4520</v>
+      </c>
+      <c r="R39" s="28">
+        <f>2*P39</f>
+        <v>2260</v>
+      </c>
+      <c r="S39" s="29">
+        <f t="shared" ref="S39:S43" si="6">Q39+R39</f>
+        <v>6780</v>
+      </c>
+      <c r="T39" s="28">
+        <v>3780</v>
+      </c>
+      <c r="U39" s="28">
+        <v>936</v>
+      </c>
+      <c r="V39" s="29">
+        <f t="shared" ref="V39:V43" si="7">T39+U39</f>
+        <v>4716</v>
+      </c>
+      <c r="W39" s="30">
+        <f t="shared" ref="W39:X43" si="8">T39/Q39</f>
+        <v>0.83628318584070793</v>
+      </c>
+      <c r="X39" s="30">
+        <f t="shared" si="8"/>
+        <v>0.41415929203539825</v>
+      </c>
+      <c r="Y39" s="31">
+        <f t="shared" ref="Y39:Y43" si="9">V39/S39</f>
+        <v>0.695575221238938</v>
+      </c>
     </row>
-    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>1330</v>
       </c>
@@ -3240,8 +3949,45 @@
         <v>24.170999999999999</v>
       </c>
       <c r="O40" s="36"/>
+      <c r="P40" s="22">
+        <v>1330</v>
+      </c>
+      <c r="Q40" s="28">
+        <f t="shared" si="5"/>
+        <v>5320</v>
+      </c>
+      <c r="R40" s="28">
+        <f t="shared" ref="R40:R43" si="10">2*P40</f>
+        <v>2660</v>
+      </c>
+      <c r="S40" s="29">
+        <f t="shared" si="6"/>
+        <v>7980</v>
+      </c>
+      <c r="T40" s="28">
+        <v>4740</v>
+      </c>
+      <c r="U40" s="28">
+        <v>632</v>
+      </c>
+      <c r="V40" s="29">
+        <f t="shared" si="7"/>
+        <v>5372</v>
+      </c>
+      <c r="W40" s="30">
+        <f t="shared" si="8"/>
+        <v>0.89097744360902253</v>
+      </c>
+      <c r="X40" s="30">
+        <f t="shared" si="8"/>
+        <v>0.23759398496240602</v>
+      </c>
+      <c r="Y40" s="31">
+        <f t="shared" si="9"/>
+        <v>0.67318295739348366</v>
+      </c>
     </row>
-    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
         <v>1530</v>
       </c>
@@ -3292,8 +4038,45 @@
         <v>23.297799999999999</v>
       </c>
       <c r="O41" s="36"/>
+      <c r="P41" s="22">
+        <v>1530</v>
+      </c>
+      <c r="Q41" s="28">
+        <f t="shared" si="5"/>
+        <v>6120</v>
+      </c>
+      <c r="R41" s="28">
+        <f t="shared" si="10"/>
+        <v>3060</v>
+      </c>
+      <c r="S41" s="29">
+        <f t="shared" si="6"/>
+        <v>9180</v>
+      </c>
+      <c r="T41" s="28">
+        <v>4884</v>
+      </c>
+      <c r="U41" s="28">
+        <v>507</v>
+      </c>
+      <c r="V41" s="29">
+        <f t="shared" si="7"/>
+        <v>5391</v>
+      </c>
+      <c r="W41" s="30">
+        <f t="shared" si="8"/>
+        <v>0.79803921568627456</v>
+      </c>
+      <c r="X41" s="30">
+        <f t="shared" si="8"/>
+        <v>0.16568627450980392</v>
+      </c>
+      <c r="Y41" s="31">
+        <f t="shared" si="9"/>
+        <v>0.58725490196078434</v>
+      </c>
     </row>
-    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>1730</v>
       </c>
@@ -3344,8 +4127,45 @@
         <v>23.216799999999999</v>
       </c>
       <c r="O42" s="36"/>
+      <c r="P42" s="22">
+        <v>1730</v>
+      </c>
+      <c r="Q42" s="28">
+        <f t="shared" si="5"/>
+        <v>6920</v>
+      </c>
+      <c r="R42" s="28">
+        <f t="shared" si="10"/>
+        <v>3460</v>
+      </c>
+      <c r="S42" s="29">
+        <f t="shared" si="6"/>
+        <v>10380</v>
+      </c>
+      <c r="T42" s="28">
+        <v>5705</v>
+      </c>
+      <c r="U42" s="28">
+        <v>305</v>
+      </c>
+      <c r="V42" s="29">
+        <f t="shared" si="7"/>
+        <v>6010</v>
+      </c>
+      <c r="W42" s="30">
+        <f t="shared" si="8"/>
+        <v>0.82442196531791911</v>
+      </c>
+      <c r="X42" s="30">
+        <f t="shared" si="8"/>
+        <v>8.8150289017341038E-2</v>
+      </c>
+      <c r="Y42" s="31">
+        <f t="shared" si="9"/>
+        <v>0.57899807321772645</v>
+      </c>
     </row>
-    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="23">
         <v>1930</v>
       </c>
@@ -3396,8 +4216,45 @@
         <v>23.014500000000002</v>
       </c>
       <c r="O43" s="36"/>
+      <c r="P43" s="23">
+        <v>1930</v>
+      </c>
+      <c r="Q43" s="32">
+        <f t="shared" si="5"/>
+        <v>7720</v>
+      </c>
+      <c r="R43" s="32">
+        <f t="shared" si="10"/>
+        <v>3860</v>
+      </c>
+      <c r="S43" s="33">
+        <f t="shared" si="6"/>
+        <v>11580</v>
+      </c>
+      <c r="T43" s="32">
+        <v>6287</v>
+      </c>
+      <c r="U43" s="32">
+        <v>144</v>
+      </c>
+      <c r="V43" s="33">
+        <f t="shared" si="7"/>
+        <v>6431</v>
+      </c>
+      <c r="W43" s="34">
+        <f t="shared" si="8"/>
+        <v>0.81437823834196887</v>
+      </c>
+      <c r="X43" s="34">
+        <f t="shared" si="8"/>
+        <v>3.7305699481865282E-2</v>
+      </c>
+      <c r="Y43" s="35">
+        <f t="shared" si="9"/>
+        <v>0.55535405872193433</v>
+      </c>
     </row>
-    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -3413,306 +4270,1335 @@
       <c r="M44" s="14"/>
       <c r="N44" s="14"/>
     </row>
-    <row r="45" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P45" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" s="38"/>
+      <c r="N46" s="39"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="40" t="s">
+      <c r="R46" s="38"/>
+      <c r="S46" s="41"/>
+      <c r="T46" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="38"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="40" t="s">
+      <c r="U46" s="38"/>
+      <c r="V46" s="41"/>
+      <c r="W46" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="39"/>
+      <c r="X46" s="38"/>
+      <c r="Y46" s="39"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N47" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="P47" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q47" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="R47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="S47" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="T47" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="U47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="26" t="s">
+      <c r="V47" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="W47" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="X47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J47" s="27" t="s">
+      <c r="Y47" s="27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
         <v>930</v>
       </c>
-      <c r="B48" s="28">
-        <f>4*A48</f>
+      <c r="B48" s="14">
+        <v>62.548000000000002</v>
+      </c>
+      <c r="C48" s="14">
+        <v>60.86</v>
+      </c>
+      <c r="D48" s="14">
+        <v>60.008000000000003</v>
+      </c>
+      <c r="E48" s="15">
+        <f>AVERAGE(B48:D48)</f>
+        <v>61.138666666666666</v>
+      </c>
+      <c r="F48" s="15">
+        <f>_xlfn.STDEV.P(B48:D48)</f>
+        <v>1.0555066187486566</v>
+      </c>
+      <c r="G48" s="10">
+        <f t="shared" ref="G48:G53" si="11">B48-L48</f>
+        <v>37.225000000000001</v>
+      </c>
+      <c r="H48" s="14">
+        <f t="shared" ref="H48:H53" si="12">C48-M48</f>
+        <v>36.646000000000001</v>
+      </c>
+      <c r="I48" s="14">
+        <f t="shared" ref="I48:I53" si="13">D48-N48</f>
+        <v>36.566000000000003</v>
+      </c>
+      <c r="J48" s="15">
+        <f>AVERAGE(G48:I48)</f>
+        <v>36.812333333333335</v>
+      </c>
+      <c r="K48" s="11">
+        <f>_xlfn.STDEV.P(G48:I48)</f>
+        <v>0.29362144941328017</v>
+      </c>
+      <c r="L48" s="12">
+        <v>25.323</v>
+      </c>
+      <c r="M48" s="14">
+        <v>24.213999999999999</v>
+      </c>
+      <c r="N48" s="13">
+        <v>23.442</v>
+      </c>
+      <c r="P48" s="22">
+        <v>930</v>
+      </c>
+      <c r="Q48" s="28">
+        <f>4*P48</f>
         <v>3720</v>
       </c>
-      <c r="C48" s="28">
-        <f>2*A48</f>
+      <c r="R48" s="28">
+        <f>2*P48</f>
         <v>1860</v>
       </c>
-      <c r="D48" s="29">
-        <f>B48+C48</f>
+      <c r="S48" s="29">
+        <f>Q48+R48</f>
         <v>5580</v>
       </c>
-      <c r="E48" s="28">
+      <c r="T48" s="28">
         <v>2964</v>
       </c>
-      <c r="F48" s="28">
+      <c r="U48" s="28">
         <v>1264</v>
       </c>
-      <c r="G48" s="29">
-        <f>E48+F48</f>
+      <c r="V48" s="29">
+        <f>T48+U48</f>
         <v>4228</v>
       </c>
-      <c r="H48" s="30">
-        <f>E48/B48</f>
+      <c r="W48" s="30">
+        <f>T48/Q48</f>
         <v>0.79677419354838708</v>
       </c>
-      <c r="I48" s="30">
-        <f>F48/C48</f>
+      <c r="X48" s="30">
+        <f>U48/R48</f>
         <v>0.67956989247311828</v>
       </c>
-      <c r="J48" s="31">
-        <f>G48/D48</f>
+      <c r="Y48" s="31">
+        <f>V48/S48</f>
         <v>0.75770609318996418</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="22">
         <v>1130</v>
       </c>
-      <c r="B49" s="28">
-        <f t="shared" ref="B49:B53" si="5">4*A49</f>
+      <c r="B49" s="14">
+        <v>58.752000000000002</v>
+      </c>
+      <c r="C49" s="14">
+        <v>58.616</v>
+      </c>
+      <c r="D49" s="14">
+        <v>57.32</v>
+      </c>
+      <c r="E49" s="15">
+        <f t="shared" ref="E49:E53" si="14">AVERAGE(B49:D49)</f>
+        <v>58.229333333333329</v>
+      </c>
+      <c r="F49" s="15">
+        <f t="shared" ref="F49:F53" si="15">_xlfn.STDEV.P(B49:D49)</f>
+        <v>0.64538842740029267</v>
+      </c>
+      <c r="G49" s="10">
+        <f t="shared" si="11"/>
+        <v>32.478800000000007</v>
+      </c>
+      <c r="H49" s="14">
+        <f t="shared" si="12"/>
+        <v>34.074000000000098</v>
+      </c>
+      <c r="I49" s="14">
+        <f t="shared" si="13"/>
+        <v>33.837400000000002</v>
+      </c>
+      <c r="J49" s="15">
+        <f t="shared" ref="J49:J53" si="16">AVERAGE(G49:I49)</f>
+        <v>33.463400000000036</v>
+      </c>
+      <c r="K49" s="11">
+        <f t="shared" ref="K49:K53" si="17">_xlfn.STDEV.P(G49:I49)</f>
+        <v>0.70288584184538994</v>
+      </c>
+      <c r="L49" s="12">
+        <v>26.273199999999999</v>
+      </c>
+      <c r="M49" s="14">
+        <v>24.541999999999899</v>
+      </c>
+      <c r="N49" s="13">
+        <v>23.482600000000001</v>
+      </c>
+      <c r="O49" s="36"/>
+      <c r="P49" s="22">
+        <v>1130</v>
+      </c>
+      <c r="Q49" s="28">
+        <f t="shared" ref="Q49:Q53" si="18">4*P49</f>
         <v>4520</v>
       </c>
-      <c r="C49" s="28">
-        <f>2*A49</f>
+      <c r="R49" s="28">
+        <f>2*P49</f>
         <v>2260</v>
       </c>
-      <c r="D49" s="29">
-        <f t="shared" ref="D49:D53" si="6">B49+C49</f>
+      <c r="S49" s="29">
+        <f t="shared" ref="S49:S53" si="19">Q49+R49</f>
         <v>6780</v>
       </c>
-      <c r="E49" s="28">
-        <v>3780</v>
-      </c>
-      <c r="F49" s="28">
-        <v>936</v>
-      </c>
-      <c r="G49" s="29">
-        <f t="shared" ref="G49:G53" si="7">E49+F49</f>
-        <v>4716</v>
-      </c>
-      <c r="H49" s="30">
-        <f t="shared" ref="H49:I53" si="8">E49/B49</f>
-        <v>0.83628318584070793</v>
-      </c>
-      <c r="I49" s="30">
-        <f t="shared" si="8"/>
-        <v>0.41415929203539825</v>
-      </c>
-      <c r="J49" s="31">
-        <f t="shared" ref="J49:J53" si="9">G49/D49</f>
-        <v>0.695575221238938</v>
+      <c r="T49" s="28">
+        <v>2964</v>
+      </c>
+      <c r="U49" s="28">
+        <v>1264</v>
+      </c>
+      <c r="V49" s="29">
+        <f t="shared" ref="V49:V53" si="20">T49+U49</f>
+        <v>4228</v>
+      </c>
+      <c r="W49" s="30">
+        <f t="shared" ref="W49:W53" si="21">T49/Q49</f>
+        <v>0.65575221238938053</v>
+      </c>
+      <c r="X49" s="30">
+        <f t="shared" ref="X49:X53" si="22">U49/R49</f>
+        <v>0.55929203539823014</v>
+      </c>
+      <c r="Y49" s="31">
+        <f t="shared" ref="Y49:Y53" si="23">V49/S49</f>
+        <v>0.62359882005899703</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
         <v>1330</v>
       </c>
-      <c r="B50" s="28">
-        <f t="shared" si="5"/>
+      <c r="B50" s="36">
+        <v>59.176000000000002</v>
+      </c>
+      <c r="C50" s="36">
+        <v>56.6</v>
+      </c>
+      <c r="D50" s="36">
+        <v>55.584000000000003</v>
+      </c>
+      <c r="E50" s="15">
+        <f t="shared" si="14"/>
+        <v>57.120000000000005</v>
+      </c>
+      <c r="F50" s="15">
+        <f t="shared" si="15"/>
+        <v>1.511823622869634</v>
+      </c>
+      <c r="G50" s="10">
+        <f t="shared" si="11"/>
+        <v>32.4998</v>
+      </c>
+      <c r="H50" s="14">
+        <f t="shared" si="12"/>
+        <v>32.214200000000105</v>
+      </c>
+      <c r="I50" s="14">
+        <f t="shared" si="13"/>
+        <v>32.191600000000008</v>
+      </c>
+      <c r="J50" s="15">
+        <f t="shared" si="16"/>
+        <v>32.301866666666704</v>
+      </c>
+      <c r="K50" s="11">
+        <f t="shared" si="17"/>
+        <v>0.14026378324030128</v>
+      </c>
+      <c r="L50" s="12">
+        <v>26.676200000000001</v>
+      </c>
+      <c r="M50" s="36">
+        <v>24.3857999999999</v>
+      </c>
+      <c r="N50" s="13">
+        <v>23.392399999999999</v>
+      </c>
+      <c r="O50" s="36"/>
+      <c r="P50" s="22">
+        <v>1330</v>
+      </c>
+      <c r="Q50" s="28">
+        <f t="shared" si="18"/>
         <v>5320</v>
       </c>
-      <c r="C50" s="28">
-        <f t="shared" ref="C50:C53" si="10">2*A50</f>
+      <c r="R50" s="28">
+        <f t="shared" ref="R50:R53" si="24">2*P50</f>
         <v>2660</v>
       </c>
-      <c r="D50" s="29">
-        <f t="shared" si="6"/>
+      <c r="S50" s="29">
+        <f t="shared" si="19"/>
         <v>7980</v>
       </c>
-      <c r="E50" s="28">
-        <v>4740</v>
-      </c>
-      <c r="F50" s="28">
-        <v>632</v>
-      </c>
-      <c r="G50" s="29">
-        <f t="shared" si="7"/>
-        <v>5372</v>
-      </c>
-      <c r="H50" s="30">
-        <f t="shared" si="8"/>
-        <v>0.89097744360902253</v>
-      </c>
-      <c r="I50" s="30">
-        <f t="shared" si="8"/>
-        <v>0.23759398496240602</v>
-      </c>
-      <c r="J50" s="31">
-        <f t="shared" si="9"/>
-        <v>0.67318295739348366</v>
+      <c r="T50" s="28">
+        <v>2964</v>
+      </c>
+      <c r="U50" s="28">
+        <v>1264</v>
+      </c>
+      <c r="V50" s="29">
+        <f t="shared" si="20"/>
+        <v>4228</v>
+      </c>
+      <c r="W50" s="30">
+        <f t="shared" si="21"/>
+        <v>0.55714285714285716</v>
+      </c>
+      <c r="X50" s="30">
+        <f t="shared" si="22"/>
+        <v>0.47518796992481205</v>
+      </c>
+      <c r="Y50" s="31">
+        <f t="shared" si="23"/>
+        <v>0.52982456140350875</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="22">
         <v>1530</v>
       </c>
-      <c r="B51" s="28">
-        <f t="shared" si="5"/>
+      <c r="B51" s="14">
+        <v>57.828000000000003</v>
+      </c>
+      <c r="C51" s="14">
+        <v>55.264000000000003</v>
+      </c>
+      <c r="D51" s="14">
+        <v>53.972000000000001</v>
+      </c>
+      <c r="E51" s="15">
+        <f t="shared" si="14"/>
+        <v>55.688000000000009</v>
+      </c>
+      <c r="F51" s="15">
+        <f t="shared" si="15"/>
+        <v>1.6025013780545301</v>
+      </c>
+      <c r="G51" s="10">
+        <f t="shared" si="11"/>
+        <v>30.600200000000005</v>
+      </c>
+      <c r="H51" s="14">
+        <f t="shared" si="12"/>
+        <v>30.809800000000003</v>
+      </c>
+      <c r="I51" s="14">
+        <f t="shared" si="13"/>
+        <v>30.648</v>
+      </c>
+      <c r="J51" s="15">
+        <f t="shared" si="16"/>
+        <v>30.686000000000003</v>
+      </c>
+      <c r="K51" s="11">
+        <f t="shared" si="17"/>
+        <v>8.9688497961927335E-2</v>
+      </c>
+      <c r="L51" s="12">
+        <v>27.227799999999998</v>
+      </c>
+      <c r="M51" s="14">
+        <v>24.4542</v>
+      </c>
+      <c r="N51" s="13">
+        <v>23.324000000000002</v>
+      </c>
+      <c r="O51" s="36"/>
+      <c r="P51" s="22">
+        <v>1530</v>
+      </c>
+      <c r="Q51" s="28">
+        <f t="shared" si="18"/>
         <v>6120</v>
       </c>
-      <c r="C51" s="28">
-        <f t="shared" si="10"/>
+      <c r="R51" s="28">
+        <f t="shared" si="24"/>
         <v>3060</v>
       </c>
-      <c r="D51" s="29">
-        <f t="shared" si="6"/>
+      <c r="S51" s="29">
+        <f t="shared" si="19"/>
         <v>9180</v>
       </c>
-      <c r="E51" s="28">
-        <v>4884</v>
-      </c>
-      <c r="F51" s="28">
-        <v>507</v>
-      </c>
-      <c r="G51" s="29">
-        <f t="shared" si="7"/>
-        <v>5391</v>
-      </c>
-      <c r="H51" s="30">
-        <f t="shared" si="8"/>
-        <v>0.79803921568627456</v>
-      </c>
-      <c r="I51" s="30">
-        <f t="shared" si="8"/>
-        <v>0.16568627450980392</v>
-      </c>
-      <c r="J51" s="31">
-        <f t="shared" si="9"/>
-        <v>0.58725490196078434</v>
+      <c r="T51" s="28">
+        <v>2964</v>
+      </c>
+      <c r="U51" s="28">
+        <v>1264</v>
+      </c>
+      <c r="V51" s="29">
+        <f t="shared" si="20"/>
+        <v>4228</v>
+      </c>
+      <c r="W51" s="30">
+        <f t="shared" si="21"/>
+        <v>0.48431372549019608</v>
+      </c>
+      <c r="X51" s="30">
+        <f t="shared" si="22"/>
+        <v>0.41307189542483658</v>
+      </c>
+      <c r="Y51" s="31">
+        <f t="shared" si="23"/>
+        <v>0.46056644880174291</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
         <v>1730</v>
       </c>
-      <c r="B52" s="28">
-        <f t="shared" si="5"/>
+      <c r="B52" s="14">
+        <v>55.911999999999999</v>
+      </c>
+      <c r="C52" s="14">
+        <v>54.148000000000003</v>
+      </c>
+      <c r="D52" s="14">
+        <v>52.874000000000002</v>
+      </c>
+      <c r="E52" s="15">
+        <f t="shared" si="14"/>
+        <v>54.31133333333333</v>
+      </c>
+      <c r="F52" s="15">
+        <f t="shared" si="15"/>
+        <v>1.2456241630425897</v>
+      </c>
+      <c r="G52" s="10">
+        <f t="shared" si="11"/>
+        <v>29.816599999999998</v>
+      </c>
+      <c r="H52" s="14">
+        <f t="shared" si="12"/>
+        <v>29.837400000000002</v>
+      </c>
+      <c r="I52" s="14">
+        <f t="shared" si="13"/>
+        <v>29.545600000000004</v>
+      </c>
+      <c r="J52" s="15">
+        <f t="shared" si="16"/>
+        <v>29.7332</v>
+      </c>
+      <c r="K52" s="11">
+        <f t="shared" si="17"/>
+        <v>0.13292474061161907</v>
+      </c>
+      <c r="L52" s="12">
+        <v>26.095400000000001</v>
+      </c>
+      <c r="M52" s="14">
+        <v>24.310600000000001</v>
+      </c>
+      <c r="N52" s="13">
+        <v>23.328399999999998</v>
+      </c>
+      <c r="O52" s="36"/>
+      <c r="P52" s="22">
+        <v>1730</v>
+      </c>
+      <c r="Q52" s="28">
+        <f t="shared" si="18"/>
         <v>6920</v>
       </c>
-      <c r="C52" s="28">
-        <f t="shared" si="10"/>
+      <c r="R52" s="28">
+        <f t="shared" si="24"/>
         <v>3460</v>
       </c>
-      <c r="D52" s="29">
-        <f t="shared" si="6"/>
+      <c r="S52" s="29">
+        <f t="shared" si="19"/>
         <v>10380</v>
       </c>
-      <c r="E52" s="28">
-        <v>5705</v>
-      </c>
-      <c r="F52" s="28">
-        <v>305</v>
-      </c>
-      <c r="G52" s="29">
-        <f t="shared" si="7"/>
-        <v>6010</v>
-      </c>
-      <c r="H52" s="30">
-        <f t="shared" si="8"/>
-        <v>0.82442196531791911</v>
-      </c>
-      <c r="I52" s="30">
-        <f t="shared" si="8"/>
-        <v>8.8150289017341038E-2</v>
-      </c>
-      <c r="J52" s="31">
-        <f t="shared" si="9"/>
-        <v>0.57899807321772645</v>
+      <c r="T52" s="28">
+        <v>2964</v>
+      </c>
+      <c r="U52" s="28">
+        <v>1264</v>
+      </c>
+      <c r="V52" s="29">
+        <f t="shared" si="20"/>
+        <v>4228</v>
+      </c>
+      <c r="W52" s="30">
+        <f t="shared" si="21"/>
+        <v>0.4283236994219653</v>
+      </c>
+      <c r="X52" s="30">
+        <f t="shared" si="22"/>
+        <v>0.36531791907514449</v>
+      </c>
+      <c r="Y52" s="31">
+        <f t="shared" si="23"/>
+        <v>0.40732177263969171</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23">
         <v>1930</v>
       </c>
-      <c r="B53" s="32">
-        <f t="shared" si="5"/>
+      <c r="B53" s="16">
+        <v>54.756</v>
+      </c>
+      <c r="C53" s="16">
+        <v>53.28</v>
+      </c>
+      <c r="D53" s="16">
+        <v>51.975999999999999</v>
+      </c>
+      <c r="E53" s="17">
+        <f t="shared" si="14"/>
+        <v>53.337333333333333</v>
+      </c>
+      <c r="F53" s="17">
+        <f t="shared" si="15"/>
+        <v>1.1356540944417113</v>
+      </c>
+      <c r="G53" s="18">
+        <f t="shared" si="11"/>
+        <v>29.062000000000001</v>
+      </c>
+      <c r="H53" s="16">
+        <f t="shared" si="12"/>
+        <v>29.029600000000002</v>
+      </c>
+      <c r="I53" s="16">
+        <f t="shared" si="13"/>
+        <v>28.6158</v>
+      </c>
+      <c r="J53" s="17">
+        <f t="shared" si="16"/>
+        <v>28.902466666666669</v>
+      </c>
+      <c r="K53" s="19">
+        <f t="shared" si="17"/>
+        <v>0.2031350508624476</v>
+      </c>
+      <c r="L53" s="20">
+        <v>25.693999999999999</v>
+      </c>
+      <c r="M53" s="16">
+        <v>24.250399999999999</v>
+      </c>
+      <c r="N53" s="21">
+        <v>23.360199999999999</v>
+      </c>
+      <c r="O53" s="36"/>
+      <c r="P53" s="23">
+        <v>1930</v>
+      </c>
+      <c r="Q53" s="32">
+        <f t="shared" si="18"/>
         <v>7720</v>
       </c>
-      <c r="C53" s="32">
-        <f t="shared" si="10"/>
+      <c r="R53" s="32">
+        <f t="shared" si="24"/>
         <v>3860</v>
       </c>
-      <c r="D53" s="33">
-        <f t="shared" si="6"/>
+      <c r="S53" s="33">
+        <f t="shared" si="19"/>
         <v>11580</v>
       </c>
-      <c r="E53" s="32">
-        <v>6287</v>
-      </c>
-      <c r="F53" s="32">
-        <v>144</v>
-      </c>
-      <c r="G53" s="33">
-        <f t="shared" si="7"/>
-        <v>6431</v>
-      </c>
-      <c r="H53" s="34">
-        <f t="shared" si="8"/>
-        <v>0.81437823834196887</v>
-      </c>
-      <c r="I53" s="34">
-        <f t="shared" si="8"/>
-        <v>3.7305699481865282E-2</v>
-      </c>
-      <c r="J53" s="35">
-        <f t="shared" si="9"/>
-        <v>0.55535405872193433</v>
+      <c r="T53" s="32">
+        <v>2964</v>
+      </c>
+      <c r="U53" s="32">
+        <v>1264</v>
+      </c>
+      <c r="V53" s="33">
+        <f t="shared" si="20"/>
+        <v>4228</v>
+      </c>
+      <c r="W53" s="34">
+        <f t="shared" si="21"/>
+        <v>0.38393782383419689</v>
+      </c>
+      <c r="X53" s="34">
+        <f t="shared" si="22"/>
+        <v>0.32746113989637304</v>
+      </c>
+      <c r="Y53" s="35">
+        <f t="shared" si="23"/>
+        <v>0.36511226252158896</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="M56" s="38"/>
+      <c r="N56" s="39"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="R56" s="38"/>
+      <c r="S56" s="41"/>
+      <c r="T56" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="U56" s="38"/>
+      <c r="V56" s="41"/>
+      <c r="W56" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="X56" s="38"/>
+      <c r="Y56" s="39"/>
+    </row>
+    <row r="57" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N57" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="P57" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S57" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="T57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V57" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="W57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y57" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="22">
+        <v>930</v>
+      </c>
+      <c r="B58" s="14">
+        <v>61.996000000000002</v>
+      </c>
+      <c r="C58" s="14">
+        <v>61.24</v>
+      </c>
+      <c r="D58" s="14">
+        <v>61.96</v>
+      </c>
+      <c r="E58" s="15">
+        <f>AVERAGE(B58:D58)</f>
+        <v>61.731999999999999</v>
+      </c>
+      <c r="F58" s="15">
+        <f>_xlfn.STDEV.P(B58:D58)</f>
+        <v>0.34820683508512562</v>
+      </c>
+      <c r="G58" s="10">
+        <f t="shared" ref="G58:G63" si="25">B58-L58</f>
+        <v>37.404600000000002</v>
+      </c>
+      <c r="H58" s="14">
+        <f t="shared" ref="H58:H63" si="26">C58-M58</f>
+        <v>37.659000000000006</v>
+      </c>
+      <c r="I58" s="14">
+        <f t="shared" ref="I58:I63" si="27">D58-N58</f>
+        <v>37.666600000000003</v>
+      </c>
+      <c r="J58" s="15">
+        <f>AVERAGE(G58:I58)</f>
+        <v>37.576733333333337</v>
+      </c>
+      <c r="K58" s="11">
+        <f>_xlfn.STDEV.P(G58:I58)</f>
+        <v>0.12175618624484398</v>
+      </c>
+      <c r="L58" s="12">
+        <v>24.5914</v>
+      </c>
+      <c r="M58" s="14">
+        <v>23.581</v>
+      </c>
+      <c r="N58" s="13">
+        <v>24.293399999999998</v>
+      </c>
+      <c r="P58" s="22">
+        <v>930</v>
+      </c>
+      <c r="Q58" s="28">
+        <f>4*P58</f>
+        <v>3720</v>
+      </c>
+      <c r="R58" s="28">
+        <f>2*P58</f>
+        <v>1860</v>
+      </c>
+      <c r="S58" s="29">
+        <f>Q58+R58</f>
+        <v>5580</v>
+      </c>
+      <c r="T58" s="28">
+        <v>2816</v>
+      </c>
+      <c r="U58" s="28">
+        <v>1331</v>
+      </c>
+      <c r="V58" s="29">
+        <f>T58+U58</f>
+        <v>4147</v>
+      </c>
+      <c r="W58" s="30">
+        <f>T58/Q58</f>
+        <v>0.75698924731182793</v>
+      </c>
+      <c r="X58" s="30">
+        <f>U58/R58</f>
+        <v>0.71559139784946235</v>
+      </c>
+      <c r="Y58" s="31">
+        <f>V58/S58</f>
+        <v>0.74318996415770611</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="22">
+        <v>1130</v>
+      </c>
+      <c r="B59" s="14">
+        <v>61.984000000000002</v>
+      </c>
+      <c r="C59" s="14">
+        <v>60.496000000000002</v>
+      </c>
+      <c r="D59" s="14">
+        <v>59.94</v>
+      </c>
+      <c r="E59" s="15">
+        <f t="shared" ref="E59:E63" si="28">AVERAGE(B59:D59)</f>
+        <v>60.806666666666672</v>
+      </c>
+      <c r="F59" s="15">
+        <f t="shared" ref="F59:F63" si="29">_xlfn.STDEV.P(B59:D59)</f>
+        <v>0.86289023378153829</v>
+      </c>
+      <c r="G59" s="10">
+        <f t="shared" si="25"/>
+        <v>36.7898</v>
+      </c>
+      <c r="H59" s="14">
+        <f t="shared" si="26"/>
+        <v>36.383200000000002</v>
+      </c>
+      <c r="I59" s="14">
+        <f t="shared" si="27"/>
+        <v>36.405999999999999</v>
+      </c>
+      <c r="J59" s="15">
+        <f t="shared" ref="J59:J63" si="30">AVERAGE(G59:I59)</f>
+        <v>36.526333333333334</v>
+      </c>
+      <c r="K59" s="11">
+        <f t="shared" ref="K59:K63" si="31">_xlfn.STDEV.P(G59:I59)</f>
+        <v>0.18653145102695695</v>
+      </c>
+      <c r="L59" s="12">
+        <v>25.194199999999999</v>
+      </c>
+      <c r="M59" s="14">
+        <v>24.1128</v>
+      </c>
+      <c r="N59" s="13">
+        <v>23.533999999999999</v>
+      </c>
+      <c r="O59" s="36"/>
+      <c r="P59" s="22">
+        <v>1130</v>
+      </c>
+      <c r="Q59" s="28">
+        <f t="shared" ref="Q59:Q63" si="32">4*P59</f>
+        <v>4520</v>
+      </c>
+      <c r="R59" s="28">
+        <f>2*P59</f>
+        <v>2260</v>
+      </c>
+      <c r="S59" s="29">
+        <f t="shared" ref="S59:S63" si="33">Q59+R59</f>
+        <v>6780</v>
+      </c>
+      <c r="T59" s="28">
+        <v>1083</v>
+      </c>
+      <c r="U59" s="28">
+        <v>2077</v>
+      </c>
+      <c r="V59" s="29">
+        <f t="shared" ref="V59:V63" si="34">T59+U59</f>
+        <v>3160</v>
+      </c>
+      <c r="W59" s="30">
+        <f t="shared" ref="W59:W63" si="35">T59/Q59</f>
+        <v>0.23960176991150442</v>
+      </c>
+      <c r="X59" s="30">
+        <f t="shared" ref="X59:X63" si="36">U59/R59</f>
+        <v>0.91902654867256639</v>
+      </c>
+      <c r="Y59" s="31">
+        <f t="shared" ref="Y59:Y63" si="37">V59/S59</f>
+        <v>0.46607669616519176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="22">
+        <v>1330</v>
+      </c>
+      <c r="B60" s="36">
+        <v>60.648000000000003</v>
+      </c>
+      <c r="C60" s="36">
+        <v>59.152000000000001</v>
+      </c>
+      <c r="D60" s="36">
+        <v>58.415999999999997</v>
+      </c>
+      <c r="E60" s="15">
+        <f t="shared" si="28"/>
+        <v>59.405333333333338</v>
+      </c>
+      <c r="F60" s="15">
+        <f t="shared" si="29"/>
+        <v>0.92865111257613508</v>
+      </c>
+      <c r="G60" s="10">
+        <f t="shared" si="25"/>
+        <v>35.436400000000106</v>
+      </c>
+      <c r="H60" s="14">
+        <f t="shared" si="26"/>
+        <v>35.103400000000001</v>
+      </c>
+      <c r="I60" s="14">
+        <f t="shared" si="27"/>
+        <v>34.794199999999996</v>
+      </c>
+      <c r="J60" s="15">
+        <f t="shared" si="30"/>
+        <v>35.111333333333363</v>
+      </c>
+      <c r="K60" s="11">
+        <f t="shared" si="31"/>
+        <v>0.26223705984391144</v>
+      </c>
+      <c r="L60" s="12">
+        <v>25.211599999999901</v>
+      </c>
+      <c r="M60" s="36">
+        <v>24.0486</v>
+      </c>
+      <c r="N60" s="13">
+        <v>23.6218</v>
+      </c>
+      <c r="O60" s="36"/>
+      <c r="P60" s="22">
+        <v>1330</v>
+      </c>
+      <c r="Q60" s="28">
+        <f t="shared" si="32"/>
+        <v>5320</v>
+      </c>
+      <c r="R60" s="28">
+        <f t="shared" ref="R60:R63" si="38">2*P60</f>
+        <v>2660</v>
+      </c>
+      <c r="S60" s="29">
+        <f t="shared" si="33"/>
+        <v>7980</v>
+      </c>
+      <c r="T60" s="28">
+        <v>103</v>
+      </c>
+      <c r="U60" s="28">
+        <v>2596</v>
+      </c>
+      <c r="V60" s="29">
+        <f t="shared" si="34"/>
+        <v>2699</v>
+      </c>
+      <c r="W60" s="30">
+        <f t="shared" si="35"/>
+        <v>1.9360902255639099E-2</v>
+      </c>
+      <c r="X60" s="30">
+        <f t="shared" si="36"/>
+        <v>0.97593984962406011</v>
+      </c>
+      <c r="Y60" s="31">
+        <f t="shared" si="37"/>
+        <v>0.33822055137844609</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="22">
+        <v>1530</v>
+      </c>
+      <c r="B61" s="14">
+        <v>58.368000000000002</v>
+      </c>
+      <c r="C61" s="14">
+        <v>57.212000000000003</v>
+      </c>
+      <c r="D61" s="14">
+        <v>56.887999999999998</v>
+      </c>
+      <c r="E61" s="15">
+        <f t="shared" si="28"/>
+        <v>57.489333333333342</v>
+      </c>
+      <c r="F61" s="15">
+        <f t="shared" si="29"/>
+        <v>0.63523503961569761</v>
+      </c>
+      <c r="G61" s="10">
+        <f t="shared" si="25"/>
+        <v>33.401000000000003</v>
+      </c>
+      <c r="H61" s="14">
+        <f t="shared" si="26"/>
+        <v>33.251200000000004</v>
+      </c>
+      <c r="I61" s="14">
+        <f t="shared" si="27"/>
+        <v>33.137199999999993</v>
+      </c>
+      <c r="J61" s="15">
+        <f t="shared" si="30"/>
+        <v>33.263133333333336</v>
+      </c>
+      <c r="K61" s="11">
+        <f t="shared" si="31"/>
+        <v>0.10802596395723466</v>
+      </c>
+      <c r="L61" s="12">
+        <v>24.966999999999999</v>
+      </c>
+      <c r="M61" s="14">
+        <v>23.960799999999999</v>
+      </c>
+      <c r="N61" s="13">
+        <v>23.750800000000002</v>
+      </c>
+      <c r="O61" s="36"/>
+      <c r="P61" s="22">
+        <v>1530</v>
+      </c>
+      <c r="Q61" s="28">
+        <f t="shared" si="32"/>
+        <v>6120</v>
+      </c>
+      <c r="R61" s="28">
+        <f t="shared" si="38"/>
+        <v>3060</v>
+      </c>
+      <c r="S61" s="29">
+        <f t="shared" si="33"/>
+        <v>9180</v>
+      </c>
+      <c r="T61" s="28">
+        <v>0</v>
+      </c>
+      <c r="U61" s="28">
+        <v>2659</v>
+      </c>
+      <c r="V61" s="29">
+        <f t="shared" si="34"/>
+        <v>2659</v>
+      </c>
+      <c r="W61" s="30">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="X61" s="30">
+        <f t="shared" si="36"/>
+        <v>0.86895424836601309</v>
+      </c>
+      <c r="Y61" s="31">
+        <f t="shared" si="37"/>
+        <v>0.28965141612200435</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="22">
+        <v>1730</v>
+      </c>
+      <c r="B62" s="14">
+        <v>56.896000000000001</v>
+      </c>
+      <c r="C62" s="14">
+        <v>55.868000000000002</v>
+      </c>
+      <c r="D62" s="14">
+        <v>55.823999999999998</v>
+      </c>
+      <c r="E62" s="15">
+        <f t="shared" si="28"/>
+        <v>56.196000000000005</v>
+      </c>
+      <c r="F62" s="15">
+        <f t="shared" si="29"/>
+        <v>0.49530058213842942</v>
+      </c>
+      <c r="G62" s="10">
+        <f t="shared" si="25"/>
+        <v>32.081200000000102</v>
+      </c>
+      <c r="H62" s="14">
+        <f t="shared" si="26"/>
+        <v>32.166800000000002</v>
+      </c>
+      <c r="I62" s="14">
+        <f t="shared" si="27"/>
+        <v>31.895599999999998</v>
+      </c>
+      <c r="J62" s="15">
+        <f t="shared" si="30"/>
+        <v>32.0478666666667</v>
+      </c>
+      <c r="K62" s="11">
+        <f t="shared" si="31"/>
+        <v>0.11319803688915357</v>
+      </c>
+      <c r="L62" s="12">
+        <v>24.814799999999899</v>
+      </c>
+      <c r="M62" s="14">
+        <v>23.7012</v>
+      </c>
+      <c r="N62" s="13">
+        <v>23.9284</v>
+      </c>
+      <c r="O62" s="36"/>
+      <c r="P62" s="22">
+        <v>1730</v>
+      </c>
+      <c r="Q62" s="28">
+        <f t="shared" si="32"/>
+        <v>6920</v>
+      </c>
+      <c r="R62" s="28">
+        <f t="shared" si="38"/>
+        <v>3460</v>
+      </c>
+      <c r="S62" s="29">
+        <f t="shared" si="33"/>
+        <v>10380</v>
+      </c>
+      <c r="T62" s="28">
+        <v>0</v>
+      </c>
+      <c r="U62" s="28">
+        <v>2659</v>
+      </c>
+      <c r="V62" s="29">
+        <f t="shared" si="34"/>
+        <v>2659</v>
+      </c>
+      <c r="W62" s="30">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="X62" s="30">
+        <f t="shared" si="36"/>
+        <v>0.76849710982658959</v>
+      </c>
+      <c r="Y62" s="31">
+        <f t="shared" si="37"/>
+        <v>0.25616570327552984</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="23">
+        <v>1930</v>
+      </c>
+      <c r="B63" s="16">
+        <v>55.415999999999997</v>
+      </c>
+      <c r="C63" s="16">
+        <v>54.524000000000001</v>
+      </c>
+      <c r="D63" s="16">
+        <v>54.896000000000001</v>
+      </c>
+      <c r="E63" s="17">
+        <f t="shared" si="28"/>
+        <v>54.945333333333338</v>
+      </c>
+      <c r="F63" s="17">
+        <f t="shared" si="29"/>
+        <v>0.36582448736457523</v>
+      </c>
+      <c r="G63" s="18">
+        <f t="shared" si="25"/>
+        <v>30.772999999999996</v>
+      </c>
+      <c r="H63" s="16">
+        <f t="shared" si="26"/>
+        <v>30.867800000000003</v>
+      </c>
+      <c r="I63" s="16">
+        <f t="shared" si="27"/>
+        <v>30.866200000000102</v>
+      </c>
+      <c r="J63" s="17">
+        <f t="shared" si="30"/>
+        <v>30.8356666666667</v>
+      </c>
+      <c r="K63" s="19">
+        <f t="shared" si="31"/>
+        <v>4.4316839036922746E-2</v>
+      </c>
+      <c r="L63" s="20">
+        <v>24.643000000000001</v>
+      </c>
+      <c r="M63" s="16">
+        <v>23.656199999999998</v>
+      </c>
+      <c r="N63" s="21">
+        <v>24.029799999999899</v>
+      </c>
+      <c r="O63" s="36"/>
+      <c r="P63" s="23">
+        <v>1930</v>
+      </c>
+      <c r="Q63" s="32">
+        <f t="shared" si="32"/>
+        <v>7720</v>
+      </c>
+      <c r="R63" s="32">
+        <f t="shared" si="38"/>
+        <v>3860</v>
+      </c>
+      <c r="S63" s="33">
+        <f t="shared" si="33"/>
+        <v>11580</v>
+      </c>
+      <c r="T63" s="32">
+        <v>0</v>
+      </c>
+      <c r="U63" s="32">
+        <v>2659</v>
+      </c>
+      <c r="V63" s="33">
+        <f t="shared" si="34"/>
+        <v>2659</v>
+      </c>
+      <c r="W63" s="34">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="X63" s="34">
+        <f t="shared" si="36"/>
+        <v>0.68886010362694305</v>
+      </c>
+      <c r="Y63" s="35">
+        <f t="shared" si="37"/>
+        <v>0.22962003454231433</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="18">
+    <mergeCell ref="W46:Y46"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="G56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="T56:V56"/>
+    <mergeCell ref="W56:Y56"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="T46:V46"/>
     <mergeCell ref="L36:N36"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="T36:V36"/>
+    <mergeCell ref="W36:Y36"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="G36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="97" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="74" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>